<commit_message>
alt. em requirements.txt e debug main.py
</commit_message>
<xml_diff>
--- a/album.xlsx
+++ b/album.xlsx
@@ -636,7 +636,7 @@
       </c>
       <c r="E2" s="33" t="n"/>
       <c r="F2" s="34" t="n">
-        <v>5486.1</v>
+        <v>5486.09</v>
       </c>
       <c r="G2" s="35" t="inlineStr">
         <is>
@@ -1616,7 +1616,7 @@
         </is>
       </c>
       <c r="D50" s="32" t="n">
-        <v>4.9</v>
+        <v>4.89</v>
       </c>
       <c r="E50" s="37" t="n"/>
       <c r="F50" s="33" t="n"/>

</xml_diff>